<commit_message>
update to prophet and lstm
</commit_message>
<xml_diff>
--- a/Results/erica/results_comparison.xlsx
+++ b/Results/erica/results_comparison.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericazhang/Desktop/nu/senior year/stat390/covid project/Results/erica/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0115D96-55BA-094D-B7E3-CE9847505816}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B316E817-3C8A-E14C-B9C9-3F71E40C8652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="2040" windowWidth="27440" windowHeight="16760" xr2:uid="{E2862D8B-86F9-3342-92CC-7056D5A74A54}"/>
+    <workbookView xWindow="1620" yWindow="740" windowWidth="27440" windowHeight="16760" xr2:uid="{E2862D8B-86F9-3342-92CC-7056D5A74A54}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
   <si>
     <t>ARIMA</t>
   </si>
@@ -125,7 +125,19 @@
     <t>Auto ARIMA Log</t>
   </si>
   <si>
-    <t>Prophet Single</t>
+    <t>Prophet Univariate</t>
+  </si>
+  <si>
+    <t>XGBoost</t>
+  </si>
+  <si>
+    <t>XGBoost Log</t>
+  </si>
+  <si>
+    <t>rmse_train_pred</t>
+  </si>
+  <si>
+    <t>rmse_test_pred</t>
   </si>
 </sst>
 </file>
@@ -498,15 +510,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8793AE92-7173-4C4B-B81D-70853928F844}">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.83203125" customWidth="1"/>
+    <col min="1" max="1" width="15.1640625" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
     <col min="3" max="3" width="18.6640625" customWidth="1"/>
     <col min="4" max="4" width="15.1640625" customWidth="1"/>
@@ -515,9 +527,13 @@
     <col min="7" max="7" width="15.6640625" customWidth="1"/>
     <col min="8" max="8" width="16.33203125" customWidth="1"/>
     <col min="9" max="9" width="15.6640625" customWidth="1"/>
+    <col min="10" max="10" width="16" customWidth="1"/>
+    <col min="11" max="11" width="13.83203125" customWidth="1"/>
+    <col min="12" max="12" width="14.33203125" customWidth="1"/>
+    <col min="13" max="13" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -530,8 +546,14 @@
       <c r="H1" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -559,8 +581,20 @@
       <c r="I2" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -583,13 +617,25 @@
         <v>9579.7551500000009</v>
       </c>
       <c r="H3" s="2">
-        <v>26666.810778442501</v>
+        <v>41677.527853200001</v>
       </c>
       <c r="I3" s="3">
-        <v>35896.582116235099</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+        <v>140116.80001539399</v>
+      </c>
+      <c r="J3" s="2">
+        <v>9.3374896530701908E-3</v>
+      </c>
+      <c r="K3" s="3">
+        <v>9762.80512208658</v>
+      </c>
+      <c r="L3" s="2">
+        <v>70.937440300000006</v>
+      </c>
+      <c r="M3" s="3">
+        <v>306.977191</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -612,13 +658,25 @@
         <v>1216459.68</v>
       </c>
       <c r="H4" s="2">
-        <v>26781.1594893314</v>
+        <v>44677.008451137503</v>
       </c>
       <c r="I4" s="3">
-        <v>34356.383772365698</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+        <v>138514.01332833199</v>
+      </c>
+      <c r="J4" s="2">
+        <v>8.5867710476515993E-2</v>
+      </c>
+      <c r="K4" s="3">
+        <v>12883.0201770245</v>
+      </c>
+      <c r="L4" s="2">
+        <v>98.872770399999993</v>
+      </c>
+      <c r="M4" s="3">
+        <v>1579.0477599999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -641,13 +699,25 @@
         <v>745.15902600000004</v>
       </c>
       <c r="H5" s="2">
-        <v>21449.8403960623</v>
+        <v>51885.912589712403</v>
       </c>
       <c r="I5" s="3">
-        <v>35958.829647673097</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+        <v>141628.28110913699</v>
+      </c>
+      <c r="J5" s="2">
+        <v>1.0322337757313E-2</v>
+      </c>
+      <c r="K5" s="3">
+        <v>5144.6570465559398</v>
+      </c>
+      <c r="L5" s="2">
+        <v>37.142817200000003</v>
+      </c>
+      <c r="M5" s="3">
+        <v>216.147267</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -670,13 +740,25 @@
         <v>3397.3787699999998</v>
       </c>
       <c r="H6" s="2">
-        <v>21840.2867977899</v>
+        <v>54509.409359711797</v>
       </c>
       <c r="I6" s="3">
-        <v>36766.888621023201</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+        <v>143262.91513128899</v>
+      </c>
+      <c r="J6" s="2">
+        <v>2.0252899570212399E-2</v>
+      </c>
+      <c r="K6" s="3">
+        <v>1711.82380124411</v>
+      </c>
+      <c r="L6" s="2">
+        <v>51.266564000000002</v>
+      </c>
+      <c r="M6" s="3">
+        <v>53.977918699999996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -699,13 +781,25 @@
         <v>1471.0404100000001</v>
       </c>
       <c r="H7" s="2">
-        <v>22033.3817155664</v>
+        <v>63008.158693643003</v>
       </c>
       <c r="I7" s="3">
-        <v>37077.690538716502</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+        <v>144278.24814274799</v>
+      </c>
+      <c r="J7" s="2">
+        <v>1.7219019473158199E-2</v>
+      </c>
+      <c r="K7" s="3">
+        <v>4950.6284708224903</v>
+      </c>
+      <c r="L7" s="2">
+        <v>7.0435169799999997</v>
+      </c>
+      <c r="M7" s="3">
+        <v>45.1423147</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -728,13 +822,25 @@
         <v>111.96141299999999</v>
       </c>
       <c r="H8" s="2">
-        <v>22524.377725209699</v>
+        <v>67631.024751529796</v>
       </c>
       <c r="I8" s="3">
-        <v>37919.244012268697</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+        <v>145339.34191183001</v>
+      </c>
+      <c r="J8" s="2">
+        <v>0.165530431190444</v>
+      </c>
+      <c r="K8" s="3">
+        <v>291.20854833188901</v>
+      </c>
+      <c r="L8" s="2">
+        <v>5.1476282600000003</v>
+      </c>
+      <c r="M8" s="3">
+        <v>5.9467273199999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -757,13 +863,25 @@
         <v>86407.629400000005</v>
       </c>
       <c r="H9" s="2">
-        <v>65095.112050949298</v>
+        <v>67423.530696454996</v>
       </c>
       <c r="I9" s="3">
-        <v>34879.918151791098</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+        <v>142939.14783218401</v>
+      </c>
+      <c r="J9" s="2">
+        <v>0.10534530444528201</v>
+      </c>
+      <c r="K9" s="3">
+        <v>43841.303002049899</v>
+      </c>
+      <c r="L9" s="2">
+        <v>384.21331099999998</v>
+      </c>
+      <c r="M9" s="3">
+        <v>1842.3820800000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -786,13 +904,25 @@
         <v>238106.829</v>
       </c>
       <c r="H10" s="2">
-        <v>57734.646242021001</v>
+        <v>63969.460950536501</v>
       </c>
       <c r="I10" s="3">
-        <v>34910.216022154404</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+        <v>143259.21010905001</v>
+      </c>
+      <c r="J10" s="2">
+        <v>6.1851356803114703E-2</v>
+      </c>
+      <c r="K10" s="3">
+        <v>43116.167235804904</v>
+      </c>
+      <c r="L10" s="2">
+        <v>243.12577400000001</v>
+      </c>
+      <c r="M10" s="3">
+        <v>2364.65517</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -815,13 +945,25 @@
         <v>2755.49908</v>
       </c>
       <c r="H11" s="2">
-        <v>80912.438394605793</v>
+        <v>82887.615848911795</v>
       </c>
       <c r="I11" s="3">
-        <v>37139.778628023501</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+        <v>147094.01504927201</v>
+      </c>
+      <c r="J11" s="2">
+        <v>0.230663872088021</v>
+      </c>
+      <c r="K11" s="3">
+        <v>18171.2455522458</v>
+      </c>
+      <c r="L11" s="2">
+        <v>394.512539</v>
+      </c>
+      <c r="M11" s="3">
+        <v>1671.9255000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -844,13 +986,25 @@
         <v>105646.774</v>
       </c>
       <c r="H12" s="2">
-        <v>40583.830595398402</v>
+        <v>69751.157774152904</v>
       </c>
       <c r="I12" s="3">
-        <v>35822.639776195399</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+        <v>146168.6830511</v>
+      </c>
+      <c r="J12" s="2">
+        <v>0.248335757534345</v>
+      </c>
+      <c r="K12" s="3">
+        <v>17970.499448345501</v>
+      </c>
+      <c r="L12" s="2">
+        <v>201.724493</v>
+      </c>
+      <c r="M12" s="3">
+        <v>1497.9585099999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -873,13 +1027,25 @@
         <v>383666.22100000002</v>
       </c>
       <c r="H13" s="2">
-        <v>56285.864102271596</v>
+        <v>79832.017655595802</v>
       </c>
       <c r="I13" s="3">
-        <v>47585.274550176196</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+        <v>138041.52579127299</v>
+      </c>
+      <c r="J13" s="2">
+        <v>0.64034407586491104</v>
+      </c>
+      <c r="K13" s="3">
+        <v>41599.817625524898</v>
+      </c>
+      <c r="L13" s="2">
+        <v>291.43051400000002</v>
+      </c>
+      <c r="M13" s="3">
+        <v>23808.587299999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -902,13 +1068,25 @@
         <v>5958.4009699999997</v>
       </c>
       <c r="H14" s="2">
-        <v>24828.511013000902</v>
+        <v>86543.413410036301</v>
       </c>
       <c r="I14" s="3">
-        <v>37990.826936113001</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+        <v>149682.07196088001</v>
+      </c>
+      <c r="J14" s="2">
+        <v>1.5109703946560801E-2</v>
+      </c>
+      <c r="K14" s="3">
+        <v>5405.2266570845804</v>
+      </c>
+      <c r="L14" s="2">
+        <v>62.897350799999998</v>
+      </c>
+      <c r="M14" s="3">
+        <v>628.85008700000003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -931,13 +1109,25 @@
         <v>185.04389800000001</v>
       </c>
       <c r="H15" s="2">
-        <v>26607.300553221899</v>
+        <v>95699.004922242195</v>
       </c>
       <c r="I15" s="3">
-        <v>38866.410570353597</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+        <v>152185.30436641601</v>
+      </c>
+      <c r="J15" s="2">
+        <v>3.4299973483100099E-2</v>
+      </c>
+      <c r="K15" s="3">
+        <v>737.86248092389496</v>
+      </c>
+      <c r="L15" s="2">
+        <v>11.384245999999999</v>
+      </c>
+      <c r="M15" s="3">
+        <v>6.3713751700000003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -960,13 +1150,25 @@
         <v>37.333731899999997</v>
       </c>
       <c r="H16" s="2">
-        <v>27150.531862326301</v>
+        <v>99523.447479713301</v>
       </c>
       <c r="I16" s="3">
-        <v>39311.815492170703</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+        <v>153159.01804723899</v>
+      </c>
+      <c r="J16" s="2">
+        <v>0.153891195391295</v>
+      </c>
+      <c r="K16" s="3">
+        <v>289.90803248323903</v>
+      </c>
+      <c r="L16" s="2">
+        <v>11.0537353</v>
+      </c>
+      <c r="M16" s="3">
+        <v>19.0895966</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -989,13 +1191,25 @@
         <v>733.96329400000002</v>
       </c>
       <c r="H17" s="2">
-        <v>26883.651281996001</v>
+        <v>101456.032713835</v>
       </c>
       <c r="I17" s="3">
-        <v>39262.868509829401</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+        <v>153714.824667251</v>
+      </c>
+      <c r="J17" s="2">
+        <v>6.8758502516597902E-2</v>
+      </c>
+      <c r="K17" s="3">
+        <v>2341.8566538833102</v>
+      </c>
+      <c r="L17" s="2">
+        <v>32.270944</v>
+      </c>
+      <c r="M17" s="3">
+        <v>400.34565900000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -1018,13 +1232,25 @@
         <v>19585.7984</v>
       </c>
       <c r="H18" s="2">
-        <v>34713.698470704301</v>
+        <v>93194.162723152796</v>
       </c>
       <c r="I18" s="3">
-        <v>35948.520586552702</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+        <v>150527.40904484299</v>
+      </c>
+      <c r="J18" s="2">
+        <v>0.18127153075201899</v>
+      </c>
+      <c r="K18" s="3">
+        <v>7227.1498971958399</v>
+      </c>
+      <c r="L18" s="2">
+        <v>160.63851700000001</v>
+      </c>
+      <c r="M18" s="3">
+        <v>2018.3075100000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -1047,13 +1273,25 @@
         <v>181.75428700000001</v>
       </c>
       <c r="H19" s="2">
-        <v>29956.563546787202</v>
+        <v>112532.68529446299</v>
       </c>
       <c r="I19" s="3">
-        <v>39791.863043845697</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+        <v>156048.05186667701</v>
+      </c>
+      <c r="J19" s="2">
+        <v>5.6394830429563801E-2</v>
+      </c>
+      <c r="K19" s="3">
+        <v>3187.4049337862002</v>
+      </c>
+      <c r="L19" s="2">
+        <v>6.9969263499999999</v>
+      </c>
+      <c r="M19" s="3">
+        <v>45.717674700000003</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -1076,13 +1314,25 @@
         <v>137.19432900000001</v>
       </c>
       <c r="H20" s="2">
-        <v>28914.875221429302</v>
+        <v>113758.394926279</v>
       </c>
       <c r="I20" s="3">
-        <v>40019.315057253603</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+        <v>156988.15887847301</v>
+      </c>
+      <c r="J20" s="2">
+        <v>1.8072463213376001E-2</v>
+      </c>
+      <c r="K20" s="3">
+        <v>865.33042819940601</v>
+      </c>
+      <c r="L20" s="2">
+        <v>34.140070600000001</v>
+      </c>
+      <c r="M20" s="3">
+        <v>81.31174</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -1105,13 +1355,25 @@
         <v>1176261.95</v>
       </c>
       <c r="H21" s="2">
-        <v>68457.028158137196</v>
+        <v>114646.741232175</v>
       </c>
       <c r="I21" s="3">
-        <v>35144.965291710199</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+        <v>138682.120143512</v>
+      </c>
+      <c r="J21" s="2">
+        <v>7.5158354265668203E-3</v>
+      </c>
+      <c r="K21" s="3">
+        <v>25687.8338526384</v>
+      </c>
+      <c r="L21" s="2">
+        <v>408.87440900000001</v>
+      </c>
+      <c r="M21" s="3">
+        <v>18971.8066</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -1134,13 +1396,25 @@
         <v>11.485736599999999</v>
       </c>
       <c r="H22" s="2">
-        <v>32608.174856475001</v>
+        <v>124982.208242052</v>
       </c>
       <c r="I22" s="3">
-        <v>40521.772084862299</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+        <v>159028.962953407</v>
+      </c>
+      <c r="J22" s="2">
+        <v>3.0568425007163402E-2</v>
+      </c>
+      <c r="K22" s="3">
+        <v>250.50184507433701</v>
+      </c>
+      <c r="L22" s="2">
+        <v>6.4802708300000003</v>
+      </c>
+      <c r="M22" s="3">
+        <v>1.46360958</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -1163,13 +1437,25 @@
         <v>5.9224845100000003</v>
       </c>
       <c r="H23" s="2">
-        <v>30820.609175089801</v>
+        <v>115654.995300418</v>
       </c>
       <c r="I23" s="3">
-        <v>40718.328784537203</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+        <v>160007.04796094901</v>
+      </c>
+      <c r="J23" s="2">
+        <v>0.25067158151049101</v>
+      </c>
+      <c r="K23" s="3">
+        <v>9053.5666809897393</v>
+      </c>
+      <c r="L23" s="2">
+        <v>136.85204300000001</v>
+      </c>
+      <c r="M23" s="3">
+        <v>2.52431888</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -1192,13 +1478,25 @@
         <v>2712.1698000000001</v>
       </c>
       <c r="H24" s="2">
-        <v>38431.282110850902</v>
+        <v>115815.90053112801</v>
       </c>
       <c r="I24" s="3">
-        <v>39649.570846328701</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+        <v>159000.879273258</v>
+      </c>
+      <c r="J24" s="2">
+        <v>0.170292168318711</v>
+      </c>
+      <c r="K24" s="3">
+        <v>8485.9268743282191</v>
+      </c>
+      <c r="L24" s="2">
+        <v>231.83571699999999</v>
+      </c>
+      <c r="M24" s="3">
+        <v>873.29628400000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -1221,10 +1519,22 @@
         <v>48350.040500000003</v>
       </c>
       <c r="H25" s="2">
-        <v>140498.65857832599</v>
+        <v>131954.99540117601</v>
       </c>
       <c r="I25" s="3">
-        <v>35325.372136558603</v>
+        <v>147743.66442476001</v>
+      </c>
+      <c r="J25" s="2">
+        <v>5.7527924811151702E-2</v>
+      </c>
+      <c r="K25" s="3">
+        <v>202694.93934196199</v>
+      </c>
+      <c r="L25" s="2">
+        <v>989.732078</v>
+      </c>
+      <c r="M25" s="3">
+        <v>3427.1462700000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Resolved merge conflict by incorporating both suggestions.
</commit_message>
<xml_diff>
--- a/Results/erica/results_comparison.xlsx
+++ b/Results/erica/results_comparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericazhang/Desktop/nu/senior year/stat390/covid project/Results/erica/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0339E96-72A4-8949-A903-6DEABD72EBD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8297DC3-CDDF-0246-B742-6746E0017F51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1620" yWindow="740" windowWidth="27440" windowHeight="16760" xr2:uid="{E2862D8B-86F9-3342-92CC-7056D5A74A54}"/>
+    <workbookView xWindow="1740" yWindow="1180" windowWidth="27440" windowHeight="16760" xr2:uid="{E2862D8B-86F9-3342-92CC-7056D5A74A54}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
   <si>
     <t>ARIMA</t>
   </si>
@@ -138,6 +138,12 @@
   </si>
   <si>
     <t>rmse_test_pred</t>
+  </si>
+  <si>
+    <t>LSTM</t>
+  </si>
+  <si>
+    <t>Prophet Multivariate</t>
   </si>
 </sst>
 </file>
@@ -510,10 +516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8793AE92-7173-4C4B-B81D-70853928F844}">
-  <dimension ref="A1:M25"/>
+  <dimension ref="A1:Q25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" zoomScale="110" workbookViewId="0">
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -524,16 +530,18 @@
     <col min="4" max="4" width="15.1640625" customWidth="1"/>
     <col min="5" max="5" width="14.33203125" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="7" max="7" width="15.6640625" customWidth="1"/>
-    <col min="8" max="8" width="16.33203125" customWidth="1"/>
-    <col min="9" max="9" width="15.6640625" customWidth="1"/>
-    <col min="10" max="10" width="16" customWidth="1"/>
-    <col min="11" max="11" width="13.83203125" customWidth="1"/>
-    <col min="12" max="12" width="14.33203125" customWidth="1"/>
-    <col min="13" max="13" width="15.33203125" customWidth="1"/>
+    <col min="7" max="9" width="15.6640625" customWidth="1"/>
+    <col min="10" max="10" width="21.1640625" customWidth="1"/>
+    <col min="11" max="11" width="15.6640625" customWidth="1"/>
+    <col min="12" max="12" width="16" customWidth="1"/>
+    <col min="13" max="13" width="13.83203125" customWidth="1"/>
+    <col min="14" max="14" width="14.33203125" customWidth="1"/>
+    <col min="15" max="15" width="15.33203125" customWidth="1"/>
+    <col min="16" max="16" width="14.5" customWidth="1"/>
+    <col min="17" max="17" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -547,13 +555,19 @@
         <v>29</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="P1" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -588,13 +602,25 @@
         <v>3</v>
       </c>
       <c r="L2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="N2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="O2" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="P2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -616,26 +642,22 @@
       <c r="G3" s="3">
         <v>9579.7551500000009</v>
       </c>
-      <c r="H3" s="2">
-        <v>41677.527853200001</v>
-      </c>
-      <c r="I3" s="3">
-        <v>140116.80001539399</v>
-      </c>
-      <c r="J3" s="2">
-        <v>9.3374896530701908E-3</v>
-      </c>
-      <c r="K3" s="3">
-        <v>9762.80512208658</v>
-      </c>
-      <c r="L3" s="2">
-        <v>70.937440300000006</v>
-      </c>
-      <c r="M3" s="3">
-        <v>306.977191</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="H3" s="2"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="2">
+        <v>5209.0420199999999</v>
+      </c>
+      <c r="Q3" s="3">
+        <v>9613.5772400000005</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -657,26 +679,22 @@
       <c r="G4" s="3">
         <v>1216459.68</v>
       </c>
-      <c r="H4" s="2">
-        <v>44677.008451137503</v>
-      </c>
-      <c r="I4" s="3">
-        <v>138514.01332833199</v>
-      </c>
-      <c r="J4" s="2">
-        <v>8.5867710476515993E-2</v>
-      </c>
-      <c r="K4" s="3">
-        <v>12883.0201770245</v>
-      </c>
-      <c r="L4" s="2">
-        <v>98.872770399999993</v>
-      </c>
-      <c r="M4" s="3">
-        <v>1579.0477599999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="H4" s="2"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="2">
+        <v>7587.0545199999997</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>12156.098400000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -698,26 +716,22 @@
       <c r="G5" s="3">
         <v>745.15902600000004</v>
       </c>
-      <c r="H5" s="2">
-        <v>51885.912589712403</v>
-      </c>
-      <c r="I5" s="3">
-        <v>141628.28110913699</v>
-      </c>
-      <c r="J5" s="2">
-        <v>1.0322337757313E-2</v>
-      </c>
-      <c r="K5" s="3">
-        <v>5144.6570465559398</v>
-      </c>
-      <c r="L5" s="2">
-        <v>37.142817200000003</v>
-      </c>
-      <c r="M5" s="3">
-        <v>216.147267</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="H5" s="2"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="2">
+        <v>3707.02891</v>
+      </c>
+      <c r="Q5" s="3">
+        <v>9500.3696299999992</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -739,26 +753,22 @@
       <c r="G6" s="3">
         <v>3397.3787699999998</v>
       </c>
-      <c r="H6" s="2">
-        <v>54509.409359711797</v>
-      </c>
-      <c r="I6" s="3">
-        <v>143262.91513128899</v>
-      </c>
-      <c r="J6" s="2">
-        <v>2.0252899570212399E-2</v>
-      </c>
-      <c r="K6" s="3">
-        <v>1711.82380124411</v>
-      </c>
-      <c r="L6" s="2">
-        <v>51.266564000000002</v>
-      </c>
-      <c r="M6" s="3">
-        <v>53.977918699999996</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="H6" s="2"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="2">
+        <v>2537.2388000000001</v>
+      </c>
+      <c r="Q6" s="3">
+        <v>6544.7338600000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -780,26 +790,22 @@
       <c r="G7" s="3">
         <v>1471.0404100000001</v>
       </c>
-      <c r="H7" s="2">
-        <v>63008.158693643003</v>
-      </c>
-      <c r="I7" s="3">
-        <v>144278.24814274799</v>
-      </c>
-      <c r="J7" s="2">
-        <v>1.7219019473158199E-2</v>
-      </c>
-      <c r="K7" s="3">
-        <v>4950.6284708224903</v>
-      </c>
-      <c r="L7" s="2">
-        <v>7.0435169799999997</v>
-      </c>
-      <c r="M7" s="3">
-        <v>45.1423147</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="H7" s="2"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="2">
+        <v>542.33594300000004</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>1384.0580199999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -821,26 +827,22 @@
       <c r="G8" s="3">
         <v>111.96141299999999</v>
       </c>
-      <c r="H8" s="2">
-        <v>67631.024751529796</v>
-      </c>
-      <c r="I8" s="3">
-        <v>145339.34191183001</v>
-      </c>
-      <c r="J8" s="2">
-        <v>0.165530431190444</v>
-      </c>
-      <c r="K8" s="3">
-        <v>291.20854833188901</v>
-      </c>
-      <c r="L8" s="2">
-        <v>5.1476282600000003</v>
-      </c>
-      <c r="M8" s="3">
-        <v>5.9467273199999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="H8" s="2"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="2">
+        <v>272.73759699999999</v>
+      </c>
+      <c r="Q8" s="3">
+        <v>1522.05096</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -862,26 +864,22 @@
       <c r="G9" s="3">
         <v>86407.629400000005</v>
       </c>
-      <c r="H9" s="2">
-        <v>67423.530696454996</v>
-      </c>
-      <c r="I9" s="3">
-        <v>142939.14783218401</v>
-      </c>
-      <c r="J9" s="2">
-        <v>0.10534530444528201</v>
-      </c>
-      <c r="K9" s="3">
-        <v>43841.303002049899</v>
-      </c>
-      <c r="L9" s="2">
-        <v>384.21331099999998</v>
-      </c>
-      <c r="M9" s="3">
-        <v>1842.3820800000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="H9" s="2"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="2">
+        <v>22730.3315</v>
+      </c>
+      <c r="Q9" s="3">
+        <v>49227.1558</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -903,26 +901,22 @@
       <c r="G10" s="3">
         <v>238106.829</v>
       </c>
-      <c r="H10" s="2">
-        <v>63969.460950536501</v>
-      </c>
-      <c r="I10" s="3">
-        <v>143259.21010905001</v>
-      </c>
-      <c r="J10" s="2">
-        <v>6.1851356803114703E-2</v>
-      </c>
-      <c r="K10" s="3">
-        <v>43116.167235804904</v>
-      </c>
-      <c r="L10" s="2">
-        <v>243.12577400000001</v>
-      </c>
-      <c r="M10" s="3">
-        <v>2364.65517</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="H10" s="2"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="2">
+        <v>16242.4483</v>
+      </c>
+      <c r="Q10" s="3">
+        <v>70222.479399999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -944,26 +938,22 @@
       <c r="G11" s="3">
         <v>2755.49908</v>
       </c>
-      <c r="H11" s="2">
-        <v>82887.615848911795</v>
-      </c>
-      <c r="I11" s="3">
-        <v>147094.01504927201</v>
-      </c>
-      <c r="J11" s="2">
-        <v>0.230663872088021</v>
-      </c>
-      <c r="K11" s="3">
-        <v>18171.2455522458</v>
-      </c>
-      <c r="L11" s="2">
-        <v>394.512539</v>
-      </c>
-      <c r="M11" s="3">
-        <v>1671.9255000000001</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="H11" s="2"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="2">
+        <v>20736.170900000001</v>
+      </c>
+      <c r="Q11" s="3">
+        <v>78090.538700000005</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -985,26 +975,22 @@
       <c r="G12" s="3">
         <v>105646.774</v>
       </c>
-      <c r="H12" s="2">
-        <v>69751.157774152904</v>
-      </c>
-      <c r="I12" s="3">
-        <v>146168.6830511</v>
-      </c>
-      <c r="J12" s="2">
-        <v>0.248335757534345</v>
-      </c>
-      <c r="K12" s="3">
-        <v>17970.499448345501</v>
-      </c>
-      <c r="L12" s="2">
-        <v>201.724493</v>
-      </c>
-      <c r="M12" s="3">
-        <v>1497.9585099999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="H12" s="2"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="2">
+        <v>11788.8339</v>
+      </c>
+      <c r="Q12" s="3">
+        <v>35739.326000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -1026,26 +1012,22 @@
       <c r="G13" s="3">
         <v>383666.22100000002</v>
       </c>
-      <c r="H13" s="2">
-        <v>79832.017655595802</v>
-      </c>
-      <c r="I13" s="3">
-        <v>138041.52579127299</v>
-      </c>
-      <c r="J13" s="2">
-        <v>0.64034407586491104</v>
-      </c>
-      <c r="K13" s="3">
-        <v>41599.817625524898</v>
-      </c>
-      <c r="L13" s="2">
-        <v>291.43051400000002</v>
-      </c>
-      <c r="M13" s="3">
-        <v>23808.587299999999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="H13" s="2"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="2">
+        <v>26909.258600000001</v>
+      </c>
+      <c r="Q13" s="3">
+        <v>28363.8262</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -1067,26 +1049,22 @@
       <c r="G14" s="3">
         <v>5958.4009699999997</v>
       </c>
-      <c r="H14" s="2">
-        <v>86543.413410036301</v>
-      </c>
-      <c r="I14" s="3">
-        <v>149682.07196088001</v>
-      </c>
-      <c r="J14" s="2">
-        <v>1.5109703946560801E-2</v>
-      </c>
-      <c r="K14" s="3">
-        <v>5405.2266570845804</v>
-      </c>
-      <c r="L14" s="2">
-        <v>62.897350799999998</v>
-      </c>
-      <c r="M14" s="3">
-        <v>628.85008700000003</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="H14" s="2"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="2">
+        <v>2724.4647300000001</v>
+      </c>
+      <c r="Q14" s="3">
+        <v>17772.509600000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -1108,26 +1086,22 @@
       <c r="G15" s="3">
         <v>185.04389800000001</v>
       </c>
-      <c r="H15" s="2">
-        <v>95699.004922242195</v>
-      </c>
-      <c r="I15" s="3">
-        <v>152185.30436641601</v>
-      </c>
-      <c r="J15" s="2">
-        <v>3.4299973483100099E-2</v>
-      </c>
-      <c r="K15" s="3">
-        <v>737.86248092389496</v>
-      </c>
-      <c r="L15" s="2">
-        <v>11.384245999999999</v>
-      </c>
-      <c r="M15" s="3">
-        <v>6.3713751700000003</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="H15" s="2"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="2">
+        <v>806.707942</v>
+      </c>
+      <c r="Q15" s="3">
+        <v>1746.5242699999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -1149,26 +1123,22 @@
       <c r="G16" s="3">
         <v>37.333731899999997</v>
       </c>
-      <c r="H16" s="2">
-        <v>99523.447479713301</v>
-      </c>
-      <c r="I16" s="3">
-        <v>153159.01804723899</v>
-      </c>
-      <c r="J16" s="2">
-        <v>0.153891195391295</v>
-      </c>
-      <c r="K16" s="3">
-        <v>289.90803248323903</v>
-      </c>
-      <c r="L16" s="2">
-        <v>11.0537353</v>
-      </c>
-      <c r="M16" s="3">
-        <v>19.0895966</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="H16" s="2"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="3"/>
+      <c r="P16" s="2">
+        <v>319.90491500000002</v>
+      </c>
+      <c r="Q16" s="3">
+        <v>3277.15598</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -1190,26 +1160,22 @@
       <c r="G17" s="3">
         <v>733.96329400000002</v>
       </c>
-      <c r="H17" s="2">
-        <v>101456.032713835</v>
-      </c>
-      <c r="I17" s="3">
-        <v>153714.824667251</v>
-      </c>
-      <c r="J17" s="2">
-        <v>6.8758502516597902E-2</v>
-      </c>
-      <c r="K17" s="3">
-        <v>2341.8566538833102</v>
-      </c>
-      <c r="L17" s="2">
-        <v>32.270944</v>
-      </c>
-      <c r="M17" s="3">
-        <v>400.34565900000001</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="H17" s="2"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="2">
+        <v>2221.4577899999999</v>
+      </c>
+      <c r="Q17" s="3">
+        <v>10154.715200000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -1231,26 +1197,22 @@
       <c r="G18" s="3">
         <v>19585.7984</v>
       </c>
-      <c r="H18" s="2">
-        <v>93194.162723152796</v>
-      </c>
-      <c r="I18" s="3">
-        <v>150527.40904484299</v>
-      </c>
-      <c r="J18" s="2">
-        <v>0.18127153075201899</v>
-      </c>
-      <c r="K18" s="3">
-        <v>7227.1498971958399</v>
-      </c>
-      <c r="L18" s="2">
-        <v>160.63851700000001</v>
-      </c>
-      <c r="M18" s="3">
-        <v>2018.3075100000001</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="H18" s="2"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="3"/>
+      <c r="P18" s="2">
+        <v>11843.636699999999</v>
+      </c>
+      <c r="Q18" s="3">
+        <v>77351.131999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -1272,26 +1234,22 @@
       <c r="G19" s="3">
         <v>181.75428700000001</v>
       </c>
-      <c r="H19" s="2">
-        <v>112532.68529446299</v>
-      </c>
-      <c r="I19" s="3">
-        <v>156048.05186667701</v>
-      </c>
-      <c r="J19" s="2">
-        <v>5.6394830429563801E-2</v>
-      </c>
-      <c r="K19" s="3">
-        <v>3187.4049337862002</v>
-      </c>
-      <c r="L19" s="2">
-        <v>6.9969263499999999</v>
-      </c>
-      <c r="M19" s="3">
-        <v>45.717674700000003</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="H19" s="2"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="3"/>
+      <c r="P19" s="2">
+        <v>191.328901</v>
+      </c>
+      <c r="Q19" s="3">
+        <v>1584.3480199999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -1313,26 +1271,22 @@
       <c r="G20" s="3">
         <v>137.19432900000001</v>
       </c>
-      <c r="H20" s="2">
-        <v>113758.394926279</v>
-      </c>
-      <c r="I20" s="3">
-        <v>156988.15887847301</v>
-      </c>
-      <c r="J20" s="2">
-        <v>1.8072463213376001E-2</v>
-      </c>
-      <c r="K20" s="3">
-        <v>865.33042819940601</v>
-      </c>
-      <c r="L20" s="2">
-        <v>34.140070600000001</v>
-      </c>
-      <c r="M20" s="3">
-        <v>81.31174</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="H20" s="2"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="3"/>
+      <c r="P20" s="2">
+        <v>1127.5193999999999</v>
+      </c>
+      <c r="Q20" s="3">
+        <v>6183.2615500000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -1354,26 +1308,22 @@
       <c r="G21" s="3">
         <v>1176261.95</v>
       </c>
-      <c r="H21" s="2">
-        <v>114646.741232175</v>
-      </c>
-      <c r="I21" s="3">
-        <v>138682.120143512</v>
-      </c>
-      <c r="J21" s="2">
-        <v>7.5158354265668203E-3</v>
-      </c>
-      <c r="K21" s="3">
-        <v>25687.8338526384</v>
-      </c>
-      <c r="L21" s="2">
-        <v>408.87440900000001</v>
-      </c>
-      <c r="M21" s="3">
-        <v>18971.8066</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="H21" s="2"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="3"/>
+      <c r="P21" s="2">
+        <v>28050.445199999998</v>
+      </c>
+      <c r="Q21" s="3">
+        <v>63036.984799999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -1395,26 +1345,22 @@
       <c r="G22" s="3">
         <v>11.485736599999999</v>
       </c>
-      <c r="H22" s="2">
-        <v>124982.208242052</v>
-      </c>
-      <c r="I22" s="3">
-        <v>159028.962953407</v>
-      </c>
-      <c r="J22" s="2">
-        <v>3.0568425007163402E-2</v>
-      </c>
-      <c r="K22" s="3">
-        <v>250.50184507433701</v>
-      </c>
-      <c r="L22" s="2">
-        <v>6.4802708300000003</v>
-      </c>
-      <c r="M22" s="3">
-        <v>1.46360958</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="H22" s="2"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="3"/>
+      <c r="P22" s="2">
+        <v>532.08892500000002</v>
+      </c>
+      <c r="Q22" s="3">
+        <v>1378.09656</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -1436,26 +1382,22 @@
       <c r="G23" s="3">
         <v>5.9224845100000003</v>
       </c>
-      <c r="H23" s="2">
-        <v>115654.995300418</v>
-      </c>
-      <c r="I23" s="3">
-        <v>160007.04796094901</v>
-      </c>
-      <c r="J23" s="2">
-        <v>0.25067158151049101</v>
-      </c>
-      <c r="K23" s="3">
-        <v>9053.5666809897393</v>
-      </c>
-      <c r="L23" s="2">
-        <v>136.85204300000001</v>
-      </c>
-      <c r="M23" s="3">
-        <v>2.52431888</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="H23" s="2"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="3"/>
+      <c r="P23" s="2">
+        <v>11437.1849</v>
+      </c>
+      <c r="Q23" s="3">
+        <v>17602.417300000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -1477,26 +1419,22 @@
       <c r="G24" s="3">
         <v>2712.1698000000001</v>
       </c>
-      <c r="H24" s="2">
-        <v>115815.90053112801</v>
-      </c>
-      <c r="I24" s="3">
-        <v>159000.879273258</v>
-      </c>
-      <c r="J24" s="2">
-        <v>0.170292168318711</v>
-      </c>
-      <c r="K24" s="3">
-        <v>8485.9268743282191</v>
-      </c>
-      <c r="L24" s="2">
-        <v>231.83571699999999</v>
-      </c>
-      <c r="M24" s="3">
-        <v>873.29628400000001</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="H24" s="2"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="3"/>
+      <c r="P24" s="2">
+        <v>19010.298200000001</v>
+      </c>
+      <c r="Q24" s="3">
+        <v>57821.034</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -1518,23 +1456,19 @@
       <c r="G25" s="3">
         <v>48350.040500000003</v>
       </c>
-      <c r="H25" s="2">
-        <v>131954.99540117601</v>
-      </c>
-      <c r="I25" s="3">
-        <v>147743.66442476001</v>
-      </c>
-      <c r="J25" s="2">
-        <v>5.7527924811151702E-2</v>
-      </c>
-      <c r="K25" s="3">
-        <v>202694.93934196199</v>
-      </c>
-      <c r="L25" s="2">
-        <v>989.732078</v>
-      </c>
-      <c r="M25" s="3">
-        <v>3427.1462700000002</v>
+      <c r="H25" s="2"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="3"/>
+      <c r="P25" s="2">
+        <v>51475.701200000003</v>
+      </c>
+      <c r="Q25" s="3">
+        <v>169216.61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix the error for prophet log
</commit_message>
<xml_diff>
--- a/Results/erica/results_comparison.xlsx
+++ b/Results/erica/results_comparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericazhang/Desktop/nu/senior year/stat390/covid project/Results/erica/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3364EDF4-BEEA-0742-B8A0-2311C802F3D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66EF4A29-F6A2-1245-A347-6977A08A24E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2240" yWindow="1500" windowWidth="27440" windowHeight="16760" xr2:uid="{E2862D8B-86F9-3342-92CC-7056D5A74A54}"/>
+    <workbookView xWindow="520" yWindow="1760" windowWidth="27440" windowHeight="16760" xr2:uid="{E2862D8B-86F9-3342-92CC-7056D5A74A54}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -257,7 +257,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -277,6 +277,8 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -593,8 +595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8793AE92-7173-4C4B-B81D-70853928F844}">
   <dimension ref="A1:AD30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="Z10" sqref="Z10"/>
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="110" workbookViewId="0">
+      <selection activeCell="AE16" sqref="AE16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -782,11 +784,11 @@
       <c r="I3" s="4">
         <v>2801.0400603105199</v>
       </c>
-      <c r="J3" s="3">
-        <v>10230.112927951801</v>
-      </c>
-      <c r="K3" s="4">
-        <v>1394.0441188878899</v>
+      <c r="J3" s="7">
+        <v>11640.048795017299</v>
+      </c>
+      <c r="K3" s="8">
+        <v>1442.3672403350799</v>
       </c>
       <c r="L3" s="3">
         <v>3471.5992200000001</v>
@@ -794,11 +796,11 @@
       <c r="M3" s="4">
         <v>5875.1641200000004</v>
       </c>
-      <c r="N3" s="3">
-        <v>3275.7562400000002</v>
-      </c>
-      <c r="O3" s="4">
-        <v>326.52563500000002</v>
+      <c r="N3" s="7">
+        <v>4375.6387165432398</v>
+      </c>
+      <c r="O3" s="8">
+        <v>294.12608791075598</v>
       </c>
       <c r="P3" s="3">
         <v>5775.1296700000003</v>
@@ -834,17 +836,17 @@
       </c>
       <c r="AA3" s="1">
         <f>MIN(U3,S3,Q3,O3,M3,K3,I3,G3,C3,E3)</f>
-        <v>326.52563500000002</v>
+        <v>294.12608791075598</v>
       </c>
       <c r="AB3" s="1" t="s">
         <v>37</v>
       </c>
       <c r="AC3" s="1" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="AD3" s="1">
-        <f>COUNTIF(AB3:AB25, "Prophet Multi Log")</f>
-        <v>11</v>
+        <f>COUNTIF(AB3:AB25, "XGBoost Log")</f>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.2">
@@ -875,11 +877,11 @@
       <c r="I4" s="4">
         <v>2921.3528283936298</v>
       </c>
-      <c r="J4" s="3">
-        <v>18924.046694775399</v>
-      </c>
-      <c r="K4" s="4">
-        <v>3349.2669917306398</v>
+      <c r="J4" s="7">
+        <v>18713.8670229938</v>
+      </c>
+      <c r="K4" s="8">
+        <v>3189.5772809863702</v>
       </c>
       <c r="L4" s="3">
         <v>2784.20046</v>
@@ -887,11 +889,11 @@
       <c r="M4" s="4">
         <v>8430.9814200000001</v>
       </c>
-      <c r="N4" s="3">
-        <v>9923.9331199999997</v>
-      </c>
-      <c r="O4" s="4">
-        <v>2298.7562200000002</v>
+      <c r="N4" s="7">
+        <v>9554.5310559264308</v>
+      </c>
+      <c r="O4" s="8">
+        <v>2483.5254193068599</v>
       </c>
       <c r="P4" s="3">
         <v>4562.1715000000004</v>
@@ -933,11 +935,11 @@
         <v>31</v>
       </c>
       <c r="AC4" s="1" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="AD4" s="1">
-        <f>COUNTIF(AB3:AB25, "XGBoost Log")</f>
-        <v>8</v>
+        <f>COUNTIF(AB3:AB25, "Prophet Multi Log")</f>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.2">
@@ -968,11 +970,11 @@
       <c r="I5" s="4">
         <v>5604.5787339619401</v>
       </c>
-      <c r="J5" s="3">
-        <v>4796.8089592594997</v>
-      </c>
-      <c r="K5" s="4">
-        <v>590.77226458455004</v>
+      <c r="J5" s="7">
+        <v>4241.2283195803002</v>
+      </c>
+      <c r="K5" s="8">
+        <v>589.08874187946799</v>
       </c>
       <c r="L5" s="3">
         <v>2319.9784599999998</v>
@@ -980,11 +982,11 @@
       <c r="M5" s="4">
         <v>3970.6836199999998</v>
       </c>
-      <c r="N5" s="3">
-        <v>2217.0307400000002</v>
-      </c>
-      <c r="O5" s="4">
-        <v>766.29683599999998</v>
+      <c r="N5" s="7">
+        <v>1610.20095395972</v>
+      </c>
+      <c r="O5" s="8">
+        <v>766.19208462482095</v>
       </c>
       <c r="P5" s="3">
         <v>2907.01595</v>
@@ -1061,11 +1063,11 @@
       <c r="I6" s="4">
         <v>4008.5972421268598</v>
       </c>
-      <c r="J6" s="3">
-        <v>7888.8061490905102</v>
-      </c>
-      <c r="K6" s="4">
-        <v>672.49266459053604</v>
+      <c r="J6" s="7">
+        <v>7061.8302411969598</v>
+      </c>
+      <c r="K6" s="8">
+        <v>665.018891557502</v>
       </c>
       <c r="L6" s="3">
         <v>2312.91615</v>
@@ -1073,11 +1075,11 @@
       <c r="M6" s="4">
         <v>3282.3881900000001</v>
       </c>
-      <c r="N6" s="3">
-        <v>1862.9514899999999</v>
-      </c>
-      <c r="O6" s="4">
-        <v>88.268212500000004</v>
+      <c r="N6" s="7">
+        <v>1320.69935608115</v>
+      </c>
+      <c r="O6" s="8">
+        <v>79.1475836389682</v>
       </c>
       <c r="P6" s="3">
         <v>3114.97795</v>
@@ -1113,7 +1115,7 @@
       </c>
       <c r="AA6" s="1">
         <f t="shared" si="1"/>
-        <v>88.268212500000004</v>
+        <v>79.1475836389682</v>
       </c>
       <c r="AB6" s="1" t="s">
         <v>37</v>
@@ -1154,11 +1156,11 @@
       <c r="I7" s="4">
         <v>8103.50362497273</v>
       </c>
-      <c r="J7" s="3">
-        <v>1359.2212649498399</v>
-      </c>
-      <c r="K7" s="4">
-        <v>122.37326462601099</v>
+      <c r="J7" s="7">
+        <v>559.17760748773799</v>
+      </c>
+      <c r="K7" s="8">
+        <v>121.862805571924</v>
       </c>
       <c r="L7" s="3">
         <v>1914.4812899999999</v>
@@ -1166,11 +1168,11 @@
       <c r="M7" s="4">
         <v>3355.1388499999998</v>
       </c>
-      <c r="N7" s="3">
-        <v>1011.60582</v>
-      </c>
-      <c r="O7" s="4">
-        <v>27.2644348</v>
+      <c r="N7" s="7">
+        <v>538.19131182588796</v>
+      </c>
+      <c r="O7" s="8">
+        <v>25.776792098995401</v>
       </c>
       <c r="P7" s="3">
         <v>1487.7415100000001</v>
@@ -1206,7 +1208,7 @@
       </c>
       <c r="AA7" s="1">
         <f t="shared" si="1"/>
-        <v>27.2644348</v>
+        <v>25.776792098995401</v>
       </c>
       <c r="AB7" s="1" t="s">
         <v>37</v>
@@ -1242,11 +1244,11 @@
       <c r="I8" s="4">
         <v>8531.3630243987209</v>
       </c>
-      <c r="J8" s="3">
-        <v>780.48095294912298</v>
-      </c>
-      <c r="K8" s="4">
-        <v>48.567016286068601</v>
+      <c r="J8" s="7">
+        <v>636.07062562039596</v>
+      </c>
+      <c r="K8" s="8">
+        <v>51.008770950348001</v>
       </c>
       <c r="L8" s="3">
         <v>2497.1831299999999</v>
@@ -1254,11 +1256,11 @@
       <c r="M8" s="4">
         <v>3151.66903</v>
       </c>
-      <c r="N8" s="3">
-        <v>438.90594499999997</v>
-      </c>
-      <c r="O8" s="4">
-        <v>9.1181583600000007</v>
+      <c r="N8" s="7">
+        <v>301.29557502951002</v>
+      </c>
+      <c r="O8" s="8">
+        <v>16.153573992116598</v>
       </c>
       <c r="P8" s="3">
         <v>1213.60589</v>
@@ -1288,11 +1290,11 @@
       <c r="Y8" s="1"/>
       <c r="Z8" s="1"/>
       <c r="AA8" s="1">
-        <f t="shared" si="1"/>
-        <v>9.1181583600000007</v>
+        <f>MIN(U8,S8,Q8,O8,M8,K8,I8,G8,C8,E8)</f>
+        <v>15.477264699999999</v>
       </c>
       <c r="AB8" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="AC8" s="1" t="s">
         <v>51</v>
@@ -1330,11 +1332,11 @@
       <c r="I9" s="4">
         <v>23624.084929764598</v>
       </c>
-      <c r="J9" s="3">
-        <v>50305.302864126497</v>
-      </c>
-      <c r="K9" s="4">
-        <v>2815.2200867295601</v>
+      <c r="J9" s="7">
+        <v>49385.0435693318</v>
+      </c>
+      <c r="K9" s="8">
+        <v>2913.0822126217199</v>
       </c>
       <c r="L9" s="3">
         <v>6954.26494</v>
@@ -1342,11 +1344,11 @@
       <c r="M9" s="4">
         <v>12427.6157</v>
       </c>
-      <c r="N9" s="3">
-        <v>17218.757600000001</v>
-      </c>
-      <c r="O9" s="4">
-        <v>8364.5037499999999</v>
+      <c r="N9" s="7">
+        <v>15326.5315496602</v>
+      </c>
+      <c r="O9" s="8">
+        <v>8283.2059134551491</v>
       </c>
       <c r="P9" s="3">
         <v>7810.0243399999999</v>
@@ -1382,7 +1384,7 @@
       </c>
       <c r="AA9" s="1">
         <f t="shared" si="1"/>
-        <v>2815.2200867295601</v>
+        <v>2913.0822126217199</v>
       </c>
       <c r="AB9" s="1" t="s">
         <v>36</v>
@@ -1418,11 +1420,11 @@
       <c r="I10" s="4">
         <v>22357.415049662301</v>
       </c>
-      <c r="J10" s="3">
-        <v>45541.103319902002</v>
-      </c>
-      <c r="K10" s="4">
-        <v>5198.6835805288902</v>
+      <c r="J10" s="7">
+        <v>45641.364775294001</v>
+      </c>
+      <c r="K10" s="8">
+        <v>5240.7442018894499</v>
       </c>
       <c r="L10" s="3">
         <v>5504.9610899999998</v>
@@ -1430,11 +1432,11 @@
       <c r="M10" s="4">
         <v>10846.865299999999</v>
       </c>
-      <c r="N10" s="3">
-        <v>13670.634099999999</v>
-      </c>
-      <c r="O10" s="4">
-        <v>10088.954100000001</v>
+      <c r="N10" s="7">
+        <v>13374.257255698099</v>
+      </c>
+      <c r="O10" s="8">
+        <v>10045.006854881</v>
       </c>
       <c r="P10" s="3">
         <v>5236.04835</v>
@@ -1465,10 +1467,10 @@
       <c r="Z10" s="1"/>
       <c r="AA10" s="1">
         <f t="shared" si="1"/>
-        <v>5198.6835805288902</v>
+        <v>5207.8503000000001</v>
       </c>
       <c r="AB10" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="AC10" s="1"/>
       <c r="AD10" s="1"/>
@@ -1501,11 +1503,11 @@
       <c r="I11" s="4">
         <v>31758.762204000501</v>
       </c>
-      <c r="J11" s="3">
-        <v>73199.643338337395</v>
-      </c>
-      <c r="K11" s="4">
-        <v>4046.9155210556</v>
+      <c r="J11" s="7">
+        <v>68769.600364518396</v>
+      </c>
+      <c r="K11" s="8">
+        <v>3892.6245613566398</v>
       </c>
       <c r="L11" s="3">
         <v>7777.3760899999997</v>
@@ -1513,11 +1515,11 @@
       <c r="M11" s="4">
         <v>3368.3599399999998</v>
       </c>
-      <c r="N11" s="3">
-        <v>20205.755099999998</v>
-      </c>
-      <c r="O11" s="4">
-        <v>811.63481200000001</v>
+      <c r="N11" s="7">
+        <v>17366.289475946101</v>
+      </c>
+      <c r="O11" s="8">
+        <v>698.32054889958101</v>
       </c>
       <c r="P11" s="3">
         <v>9289.4516299999996</v>
@@ -1546,7 +1548,7 @@
       </c>
       <c r="AA11" s="1">
         <f t="shared" si="1"/>
-        <v>811.63481200000001</v>
+        <v>698.32054889958101</v>
       </c>
       <c r="AB11" s="1" t="s">
         <v>37</v>
@@ -1582,11 +1584,11 @@
       <c r="I12" s="4">
         <v>12024.590610729399</v>
       </c>
-      <c r="J12" s="3">
-        <v>27522.119301880801</v>
-      </c>
-      <c r="K12" s="4">
-        <v>2737.7189401485798</v>
+      <c r="J12" s="7">
+        <v>22890.872054252199</v>
+      </c>
+      <c r="K12" s="8">
+        <v>2813.9635638904801</v>
       </c>
       <c r="L12" s="3">
         <v>3320.6957400000001</v>
@@ -1594,11 +1596,11 @@
       <c r="M12" s="4">
         <v>5789.0395699999999</v>
       </c>
-      <c r="N12" s="3">
-        <v>10861.0296</v>
-      </c>
-      <c r="O12" s="4">
-        <v>2775.3058099999998</v>
+      <c r="N12" s="7">
+        <v>8008.5196364593203</v>
+      </c>
+      <c r="O12" s="8">
+        <v>2962.7121481930799</v>
       </c>
       <c r="P12" s="3">
         <v>10911.7238</v>
@@ -1665,11 +1667,11 @@
       <c r="I13" s="4">
         <v>45615.441736389097</v>
       </c>
-      <c r="J13" s="3">
-        <v>61026.073849536602</v>
-      </c>
-      <c r="K13" s="4">
-        <v>50712.552978999498</v>
+      <c r="J13" s="7">
+        <v>45391.200597725503</v>
+      </c>
+      <c r="K13" s="8">
+        <v>38688.288493658998</v>
       </c>
       <c r="L13" s="3">
         <v>6573.6968399999996</v>
@@ -1677,11 +1679,11 @@
       <c r="M13" s="4">
         <v>7107.3751499999998</v>
       </c>
-      <c r="N13" s="3">
-        <v>22072.984499999999</v>
-      </c>
-      <c r="O13" s="4">
-        <v>7708.1646799999999</v>
+      <c r="N13" s="7">
+        <v>19799.596627865001</v>
+      </c>
+      <c r="O13" s="8">
+        <v>15031.7553117681</v>
       </c>
       <c r="P13" s="3">
         <v>15347.733399999999</v>
@@ -1746,11 +1748,11 @@
       <c r="I14" s="4">
         <v>3887.0676344955</v>
       </c>
-      <c r="J14" s="3">
-        <v>8229.1320014170306</v>
-      </c>
-      <c r="K14" s="4">
-        <v>1505.6622634630401</v>
+      <c r="J14" s="7">
+        <v>5306.9123091236697</v>
+      </c>
+      <c r="K14" s="8">
+        <v>991.32410048829195</v>
       </c>
       <c r="L14" s="3">
         <v>2898.5926100000001</v>
@@ -1758,11 +1760,11 @@
       <c r="M14" s="4">
         <v>3151.11042</v>
       </c>
-      <c r="N14" s="3">
-        <v>5269.0673500000003</v>
-      </c>
-      <c r="O14" s="4">
-        <v>562.64117299999998</v>
+      <c r="N14" s="7">
+        <v>2372.2247577135199</v>
+      </c>
+      <c r="O14" s="8">
+        <v>380.82131813057202</v>
       </c>
       <c r="P14" s="3">
         <v>3784.4539100000002</v>
@@ -1793,7 +1795,7 @@
       <c r="Z14" s="1"/>
       <c r="AA14" s="1">
         <f t="shared" si="1"/>
-        <v>562.64117299999998</v>
+        <v>380.82131813057202</v>
       </c>
       <c r="AB14" s="1" t="s">
         <v>37</v>
@@ -1829,11 +1831,11 @@
       <c r="I15" s="4">
         <v>7874.2320804050696</v>
       </c>
-      <c r="J15" s="3">
-        <v>2123.9275604423001</v>
-      </c>
-      <c r="K15" s="4">
-        <v>117.72202043539799</v>
+      <c r="J15" s="7">
+        <v>1655.6940825592801</v>
+      </c>
+      <c r="K15" s="8">
+        <v>119.242188732706</v>
       </c>
       <c r="L15" s="3">
         <v>2476.7549600000002</v>
@@ -1841,11 +1843,11 @@
       <c r="M15" s="4">
         <v>3490.2289099999998</v>
       </c>
-      <c r="N15" s="3">
-        <v>1100.0882200000001</v>
-      </c>
-      <c r="O15" s="4">
-        <v>14.196170800000001</v>
+      <c r="N15" s="7">
+        <v>634.72289807613697</v>
+      </c>
+      <c r="O15" s="8">
+        <v>17.060707557476899</v>
       </c>
       <c r="P15" s="3">
         <v>1488.75749</v>
@@ -1912,11 +1914,11 @@
       <c r="I16" s="4">
         <v>7612.1505066555101</v>
       </c>
-      <c r="J16" s="3">
-        <v>1567.2570627719299</v>
-      </c>
-      <c r="K16" s="4">
-        <v>183.040565213094</v>
+      <c r="J16" s="7">
+        <v>1509.10612757688</v>
+      </c>
+      <c r="K16" s="8">
+        <v>187.63939164019101</v>
       </c>
       <c r="L16" s="3">
         <v>2105.7239</v>
@@ -1924,11 +1926,11 @@
       <c r="M16" s="4">
         <v>3723.1724800000002</v>
       </c>
-      <c r="N16" s="3">
-        <v>738.53143999999998</v>
-      </c>
-      <c r="O16" s="4">
-        <v>31.522402400000001</v>
+      <c r="N16" s="7">
+        <v>674.40915684266997</v>
+      </c>
+      <c r="O16" s="8">
+        <v>44.240756483924798</v>
       </c>
       <c r="P16" s="3">
         <v>1453.3621900000001</v>
@@ -1995,11 +1997,11 @@
       <c r="I17" s="4">
         <v>5822.4018200573501</v>
       </c>
-      <c r="J17" s="3">
-        <v>5745.6694977625602</v>
-      </c>
-      <c r="K17" s="4">
-        <v>603.77740530737697</v>
+      <c r="J17" s="7">
+        <v>4651.5870021993696</v>
+      </c>
+      <c r="K17" s="8">
+        <v>359.60588706213599</v>
       </c>
       <c r="L17" s="3">
         <v>2723.0319</v>
@@ -2007,11 +2009,11 @@
       <c r="M17" s="4">
         <v>3837.9747299999999</v>
       </c>
-      <c r="N17" s="3">
-        <v>2751.5578700000001</v>
-      </c>
-      <c r="O17" s="4">
-        <v>356.351361</v>
+      <c r="N17" s="7">
+        <v>3725.01508956718</v>
+      </c>
+      <c r="O17" s="8">
+        <v>693.11890255844105</v>
       </c>
       <c r="P17" s="3">
         <v>2798.1460499999998</v>
@@ -2042,10 +2044,10 @@
       <c r="Z17" s="1"/>
       <c r="AA17" s="1">
         <f t="shared" si="1"/>
-        <v>356.351361</v>
+        <v>359.60588706213599</v>
       </c>
       <c r="AB17" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AC17" s="1"/>
       <c r="AD17" s="1"/>
@@ -2078,11 +2080,11 @@
       <c r="I18" s="4">
         <v>7444.1177501190004</v>
       </c>
-      <c r="J18" s="3">
-        <v>22092.113629720199</v>
-      </c>
-      <c r="K18" s="4">
-        <v>4719.0719571359396</v>
+      <c r="J18" s="7">
+        <v>22710.669437433098</v>
+      </c>
+      <c r="K18" s="8">
+        <v>4213.5943597675496</v>
       </c>
       <c r="L18" s="3">
         <v>2734.3275800000001</v>
@@ -2090,11 +2092,11 @@
       <c r="M18" s="4">
         <v>2976.9324700000002</v>
       </c>
-      <c r="N18" s="3">
-        <v>4491.9011899999996</v>
-      </c>
-      <c r="O18" s="4">
-        <v>1110.89473</v>
+      <c r="N18" s="7">
+        <v>6233.5618948253896</v>
+      </c>
+      <c r="O18" s="8">
+        <v>1404.51314515833</v>
       </c>
       <c r="P18" s="3">
         <v>5826.2499500000004</v>
@@ -2125,7 +2127,7 @@
       <c r="Z18" s="1"/>
       <c r="AA18" s="1">
         <f t="shared" si="1"/>
-        <v>1110.89473</v>
+        <v>1404.51314515833</v>
       </c>
       <c r="AB18" s="1" t="s">
         <v>37</v>
@@ -2161,11 +2163,11 @@
       <c r="I19" s="4">
         <v>8265.3423230077806</v>
       </c>
-      <c r="J19" s="3">
-        <v>991.77573375875704</v>
-      </c>
-      <c r="K19" s="4">
-        <v>111.31813522752201</v>
+      <c r="J19" s="7">
+        <v>931.44925959738396</v>
+      </c>
+      <c r="K19" s="8">
+        <v>113.530576897034</v>
       </c>
       <c r="L19" s="3">
         <v>2276.3389400000001</v>
@@ -2173,11 +2175,11 @@
       <c r="M19" s="4">
         <v>3457.88328</v>
       </c>
-      <c r="N19" s="3">
-        <v>496.63525399999997</v>
-      </c>
-      <c r="O19" s="4">
-        <v>29.087929599999999</v>
+      <c r="N19" s="7">
+        <v>451.34435807944197</v>
+      </c>
+      <c r="O19" s="8">
+        <v>40.257027483270399</v>
       </c>
       <c r="P19" s="3">
         <v>1152.98495</v>
@@ -2208,7 +2210,7 @@
       <c r="Z19" s="1"/>
       <c r="AA19" s="1">
         <f t="shared" si="1"/>
-        <v>29.087929599999999</v>
+        <v>40.257027483270399</v>
       </c>
       <c r="AB19" s="1" t="s">
         <v>37</v>
@@ -2244,11 +2246,11 @@
       <c r="I20" s="4">
         <v>5594.9950189888896</v>
       </c>
-      <c r="J20" s="3">
-        <v>6365.4750341220097</v>
-      </c>
-      <c r="K20" s="4">
-        <v>382.89734424219301</v>
+      <c r="J20" s="7">
+        <v>5277.36735552354</v>
+      </c>
+      <c r="K20" s="8">
+        <v>381.26155955361702</v>
       </c>
       <c r="L20" s="3">
         <v>2314.0991399999998</v>
@@ -2256,11 +2258,11 @@
       <c r="M20" s="4">
         <v>3152.3773700000002</v>
       </c>
-      <c r="N20" s="3">
-        <v>2630.9161600000002</v>
-      </c>
-      <c r="O20" s="4">
-        <v>57.354010100000004</v>
+      <c r="N20" s="7">
+        <v>1687.8776813662801</v>
+      </c>
+      <c r="O20" s="8">
+        <v>62.072489182427702</v>
       </c>
       <c r="P20" s="3">
         <v>3073.14192</v>
@@ -2291,7 +2293,7 @@
       <c r="Z20" s="1"/>
       <c r="AA20" s="1">
         <f t="shared" si="1"/>
-        <v>57.354010100000004</v>
+        <v>62.072489182427702</v>
       </c>
       <c r="AB20" s="1" t="s">
         <v>37</v>
@@ -2327,11 +2329,11 @@
       <c r="I21" s="4">
         <v>13895.0347863262</v>
       </c>
-      <c r="J21" s="3">
-        <v>63451.217805326101</v>
-      </c>
-      <c r="K21" s="4">
-        <v>23181.6118365078</v>
+      <c r="J21" s="7">
+        <v>65207.1795219958</v>
+      </c>
+      <c r="K21" s="8">
+        <v>21742.695777712401</v>
       </c>
       <c r="L21" s="3">
         <v>3855.1309500000002</v>
@@ -2339,11 +2341,11 @@
       <c r="M21" s="4">
         <v>10332.536700000001</v>
       </c>
-      <c r="N21" s="3">
-        <v>12656.071</v>
-      </c>
-      <c r="O21" s="4">
-        <v>21526.621800000001</v>
+      <c r="N21" s="7">
+        <v>10445.635847887699</v>
+      </c>
+      <c r="O21" s="8">
+        <v>24466.323475619</v>
       </c>
       <c r="P21" s="3">
         <v>11863.430399999999</v>
@@ -2410,11 +2412,11 @@
       <c r="I22" s="4">
         <v>8373.2626751136704</v>
       </c>
-      <c r="J22" s="3">
-        <v>1081.2818666493199</v>
-      </c>
-      <c r="K22" s="4">
-        <v>46.474793479972398</v>
+      <c r="J22" s="7">
+        <v>1010.9152728550901</v>
+      </c>
+      <c r="K22" s="8">
+        <v>46.873042041165299</v>
       </c>
       <c r="L22" s="3">
         <v>2098.8578000000002</v>
@@ -2422,11 +2424,11 @@
       <c r="M22" s="4">
         <v>3395.0609399999998</v>
       </c>
-      <c r="N22" s="3">
-        <v>263.80188600000002</v>
-      </c>
-      <c r="O22" s="4">
-        <v>3.9701797299999999</v>
+      <c r="N22" s="7">
+        <v>270.95629025490399</v>
+      </c>
+      <c r="O22" s="8">
+        <v>4.87007291642312</v>
       </c>
       <c r="P22" s="3">
         <v>1106.7934600000001</v>
@@ -2493,11 +2495,11 @@
       <c r="I23" s="4">
         <v>7948.3355368190796</v>
       </c>
-      <c r="J23" s="3">
-        <v>15992.223372664301</v>
-      </c>
-      <c r="K23" s="4">
-        <v>1862.09025478956</v>
+      <c r="J23" s="7">
+        <v>15681.449168176099</v>
+      </c>
+      <c r="K23" s="8">
+        <v>1861.09492594876</v>
       </c>
       <c r="L23" s="3">
         <v>2590.8672700000002</v>
@@ -2505,11 +2507,11 @@
       <c r="M23" s="4">
         <v>6238.08932</v>
       </c>
-      <c r="N23" s="3">
-        <v>4283.0043699999997</v>
-      </c>
-      <c r="O23" s="4">
-        <v>10.1268785</v>
+      <c r="N23" s="7">
+        <v>4156.1877357527201</v>
+      </c>
+      <c r="O23" s="8">
+        <v>9.1462157159931099</v>
       </c>
       <c r="P23" s="3">
         <v>5344.0601299999998</v>
@@ -2576,11 +2578,11 @@
       <c r="I24" s="4">
         <v>12226.7246542883</v>
       </c>
-      <c r="J24" s="3">
-        <v>28753.8565719006</v>
-      </c>
-      <c r="K24" s="4">
-        <v>1975.6090185609301</v>
+      <c r="J24" s="7">
+        <v>24285.700617437298</v>
+      </c>
+      <c r="K24" s="8">
+        <v>1958.9500414245799</v>
       </c>
       <c r="L24" s="3">
         <v>3676.3652900000002</v>
@@ -2588,11 +2590,11 @@
       <c r="M24" s="4">
         <v>5714.5949000000001</v>
       </c>
-      <c r="N24" s="3">
-        <v>10689.264800000001</v>
-      </c>
-      <c r="O24" s="4">
-        <v>2116.1873799999998</v>
+      <c r="N24" s="7">
+        <v>7895.4419769427204</v>
+      </c>
+      <c r="O24" s="8">
+        <v>2177.2254176787701</v>
       </c>
       <c r="P24" s="3">
         <v>9667.6241000000009</v>
@@ -2659,11 +2661,11 @@
       <c r="I25" s="4">
         <v>70536.669390139796</v>
       </c>
-      <c r="J25" s="3">
-        <v>94433.859675934</v>
-      </c>
-      <c r="K25" s="4">
-        <v>16276.018017791899</v>
+      <c r="J25" s="7">
+        <v>71972.075690319194</v>
+      </c>
+      <c r="K25" s="8">
+        <v>17533.522668323501</v>
       </c>
       <c r="L25" s="3">
         <v>20937.823199999999</v>
@@ -2671,11 +2673,11 @@
       <c r="M25" s="4">
         <v>7947.5723399999997</v>
       </c>
-      <c r="N25" s="3">
-        <v>113990.857</v>
-      </c>
-      <c r="O25" s="4">
-        <v>5119.3205600000001</v>
+      <c r="N25" s="7">
+        <v>131393.14026186499</v>
+      </c>
+      <c r="O25" s="8">
+        <v>6746.4428313470698</v>
       </c>
       <c r="P25" s="3">
         <v>18499.036899999999</v>
@@ -2706,7 +2708,7 @@
       <c r="Z25" s="1"/>
       <c r="AA25" s="1">
         <f t="shared" si="1"/>
-        <v>5119.3205600000001</v>
+        <v>6746.4428313470698</v>
       </c>
       <c r="AB25" s="1" t="s">
         <v>37</v>
@@ -2752,11 +2754,11 @@
       </c>
       <c r="J27" s="1">
         <f t="shared" si="2"/>
-        <v>94433.859675934</v>
+        <v>71972.075690319194</v>
       </c>
       <c r="K27" s="1">
         <f t="shared" si="2"/>
-        <v>50712.552978999498</v>
+        <v>38688.288493658998</v>
       </c>
       <c r="L27" s="1">
         <f t="shared" si="2"/>
@@ -2768,11 +2770,11 @@
       </c>
       <c r="N27" s="1">
         <f t="shared" si="2"/>
-        <v>113990.857</v>
+        <v>131393.14026186499</v>
       </c>
       <c r="O27" s="1">
-        <f t="shared" si="2"/>
-        <v>21526.621800000001</v>
+        <f>MAX(O3:O25)</f>
+        <v>24466.323475619</v>
       </c>
       <c r="P27" s="1">
         <f t="shared" si="2"/>
@@ -2900,11 +2902,11 @@
       </c>
       <c r="J29" s="1">
         <f t="shared" si="3"/>
-        <v>780.48095294912298</v>
+        <v>559.17760748773799</v>
       </c>
       <c r="K29" s="1">
         <f t="shared" si="3"/>
-        <v>46.474793479972398</v>
+        <v>46.873042041165299</v>
       </c>
       <c r="L29" s="1">
         <f t="shared" si="3"/>
@@ -2916,11 +2918,11 @@
       </c>
       <c r="N29" s="1">
         <f t="shared" si="3"/>
-        <v>263.80188600000002</v>
+        <v>270.95629025490399</v>
       </c>
       <c r="O29" s="1">
         <f t="shared" si="3"/>
-        <v>3.9701797299999999</v>
+        <v>4.87007291642312</v>
       </c>
       <c r="P29" s="1">
         <f t="shared" si="3"/>
@@ -2974,7 +2976,7 @@
         <v>4</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K30" s="1" t="s">
         <v>23</v>

</xml_diff>